<commit_message>
mini game painting (partly)
</commit_message>
<xml_diff>
--- a/Excel Table/Dialog.xlsx
+++ b/Excel Table/Dialog.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="19">
   <si>
     <t>ID</t>
   </si>
@@ -45,6 +45,9 @@
     <t>hello</t>
   </si>
   <si>
+    <t>boss</t>
+  </si>
+  <si>
     <t>Left</t>
   </si>
   <si>
@@ -54,6 +57,9 @@
     <t>how are u</t>
   </si>
   <si>
+    <t>douban_junior</t>
+  </si>
+  <si>
     <t>Right</t>
   </si>
   <si>
@@ -61,6 +67,12 @@
   </si>
   <si>
     <t>i am fine, and u</t>
+  </si>
+  <si>
+    <t>oversea_bf</t>
+  </si>
+  <si>
+    <t>Middle</t>
   </si>
 </sst>
 </file>
@@ -68,10 +80,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -90,6 +102,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -119,40 +138,71 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -167,13 +217,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -194,37 +237,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -235,43 +247,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -283,139 +421,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -426,21 +438,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -461,11 +458,50 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
       <bottom style="double">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -502,30 +538,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -534,10 +546,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -546,133 +558,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1036,7 +1048,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
+      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="6"/>
@@ -1081,8 +1093,11 @@
       <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="D2" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="E2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G2">
         <v>1002</v>
@@ -1093,13 +1108,16 @@
         <v>1002</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G3">
         <v>1003</v>
@@ -1110,13 +1128,16 @@
         <v>1003</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G4">
         <v>1004</v>
@@ -1127,13 +1148,16 @@
         <v>1004</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="D5" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="E5" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G5">
         <v>1005</v>
@@ -1144,13 +1168,16 @@
         <v>1005</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="E6" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G6">
         <v>1006</v>
@@ -1161,13 +1188,16 @@
         <v>1006</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="G7">
         <v>1007</v>
@@ -1178,13 +1208,16 @@
         <v>1007</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="D8" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="E8" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G8">
         <v>1008</v>
@@ -1195,13 +1228,16 @@
         <v>1008</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G9">
         <v>1009</v>
@@ -1212,13 +1248,16 @@
         <v>1009</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G10">
         <v>1010</v>
@@ -1229,13 +1268,16 @@
         <v>1010</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="D11" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="E11" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G11" s="1">
         <v>0</v>

</xml_diff>